<commit_message>
Sprint N°3 Montagem de Gráficos
</commit_message>
<xml_diff>
--- a/uploads/Zez_Excel.xlsx
+++ b/uploads/Zez_Excel.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27525"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27528"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4864AD09-5AF9-4B19-8744-64688FA2CBF7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B5A6BE5-A6D7-4B3C-8A2A-D8893212F8AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -226,7 +226,7 @@
   <numFmts count="1">
     <numFmt numFmtId="8" formatCode="&quot;R$&quot;\ #,##0.00;[Red]\-&quot;R$&quot;\ #,##0.00"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,11 +237,6 @@
     <font>
       <sz val="10"/>
       <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF0D0D0D"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -306,25 +301,25 @@
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="8" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="8" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -663,8 +658,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B21"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -714,662 +709,662 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" s="4">
+      <c r="A2" s="6">
         <v>45352</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="6">
+      <c r="E2" s="7">
         <v>5</v>
       </c>
-      <c r="F2" s="7">
+      <c r="F2" s="8">
         <v>100</v>
       </c>
-      <c r="G2" s="8">
+      <c r="G2" s="5">
         <f>F2*E2</f>
         <v>500</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:10">
-      <c r="A3" s="4">
+      <c r="A3" s="6">
         <v>45356</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="4">
         <v>2</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <v>10</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="8">
         <v>200</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="5">
         <f>F3*E3</f>
         <v>2000</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="4">
+      <c r="A4" s="6">
         <v>45359</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="4">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>3</v>
       </c>
-      <c r="F4" s="7">
+      <c r="F4" s="8">
         <v>120</v>
       </c>
-      <c r="G4" s="8">
+      <c r="G4" s="5">
         <f t="shared" ref="G4:G21" si="0">F4*E4</f>
         <v>360</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="I4" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J4" s="6" t="s">
+      <c r="J4" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>45363</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="4">
         <v>4</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>8</v>
       </c>
-      <c r="F5" s="7">
+      <c r="F5" s="8">
         <v>150</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="5">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="J5" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>45366</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="4">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="7">
         <v>2</v>
       </c>
-      <c r="F6" s="7">
+      <c r="F6" s="8">
         <v>120</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="5">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="I6" s="6" t="s">
+      <c r="I6" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="J6" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>45369</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="4">
         <v>6</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="7">
         <v>6</v>
       </c>
-      <c r="F7" s="7">
+      <c r="F7" s="8">
         <v>150</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="6" t="s">
+      <c r="I7" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="6" t="s">
+      <c r="J7" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>45373</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="4">
         <v>7</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="7">
         <v>4</v>
       </c>
-      <c r="F8" s="7">
+      <c r="F8" s="8">
         <v>200</v>
       </c>
-      <c r="G8" s="8">
+      <c r="G8" s="5">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="I8" s="6" t="s">
+      <c r="I8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="6" t="s">
+      <c r="J8" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="4">
+      <c r="A9" s="6">
         <v>45376</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="4">
         <v>8</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="7">
         <v>7</v>
       </c>
-      <c r="F9" s="7">
+      <c r="F9" s="8">
         <v>150</v>
       </c>
-      <c r="G9" s="8">
+      <c r="G9" s="5">
         <f t="shared" si="0"/>
         <v>1050</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="I9" s="6" t="s">
+      <c r="I9" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="6" t="s">
+      <c r="J9" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="4">
+      <c r="A10" s="6">
         <v>45379</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="4">
         <v>9</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="7">
         <v>9</v>
       </c>
-      <c r="F10" s="7">
+      <c r="F10" s="8">
         <v>100</v>
       </c>
-      <c r="G10" s="8">
+      <c r="G10" s="5">
         <f t="shared" si="0"/>
         <v>900</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="I10" s="6" t="s">
+      <c r="I10" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="6" t="s">
+      <c r="J10" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="4">
+      <c r="A11" s="6">
         <v>45384</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="4">
         <v>10</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="7">
         <v>1</v>
       </c>
-      <c r="F11" s="7">
+      <c r="F11" s="8">
         <v>120</v>
       </c>
-      <c r="G11" s="8">
+      <c r="G11" s="5">
         <f t="shared" si="0"/>
         <v>120</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="I11" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="J11" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="4">
+      <c r="A12" s="6">
         <v>45387</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="4">
         <v>11</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E12" s="6">
+      <c r="E12" s="7">
         <v>3</v>
       </c>
-      <c r="F12" s="7">
+      <c r="F12" s="8">
         <v>100</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="5">
         <f t="shared" si="0"/>
         <v>300</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="I12" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="6" t="s">
+      <c r="J12" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="4">
+      <c r="A13" s="6">
         <v>45391</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="4">
         <v>12</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="7">
         <v>6</v>
       </c>
-      <c r="F13" s="7">
+      <c r="F13" s="8">
         <v>200</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <f t="shared" si="0"/>
         <v>1200</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I13" s="6" t="s">
+      <c r="I13" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="6" t="s">
+      <c r="J13" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="4">
+      <c r="A14" s="6">
         <v>45394</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="4">
         <v>13</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="D14" s="6" t="s">
+      <c r="D14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="7">
         <v>5</v>
       </c>
-      <c r="F14" s="7">
+      <c r="F14" s="8">
         <v>150</v>
       </c>
-      <c r="G14" s="8">
+      <c r="G14" s="5">
         <f t="shared" si="0"/>
         <v>750</v>
       </c>
-      <c r="H14" s="6" t="s">
+      <c r="H14" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="I14" s="6" t="s">
+      <c r="I14" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J14" s="6" t="s">
+      <c r="J14" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="15" spans="1:10">
-      <c r="A15" s="4">
+      <c r="A15" s="6">
         <v>45398</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="4">
         <v>14</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="6">
+      <c r="E15" s="7">
         <v>4</v>
       </c>
-      <c r="F15" s="7">
+      <c r="F15" s="8">
         <v>120</v>
       </c>
-      <c r="G15" s="8">
+      <c r="G15" s="5">
         <f t="shared" si="0"/>
         <v>480</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="I15" s="6" t="s">
+      <c r="I15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J15" s="6" t="s">
+      <c r="J15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="4">
+      <c r="A16" s="6">
         <v>45401</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="4">
         <v>15</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="6">
+      <c r="E16" s="7">
         <v>7</v>
       </c>
-      <c r="F16" s="7">
+      <c r="F16" s="8">
         <v>100</v>
       </c>
-      <c r="G16" s="8">
+      <c r="G16" s="5">
         <f t="shared" si="0"/>
         <v>700</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I16" s="6" t="s">
+      <c r="I16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="6" t="s">
+      <c r="J16" s="7" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="4">
+      <c r="A17" s="6">
         <v>45405</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="4">
         <v>16</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="C17" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="D17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E17" s="6">
+      <c r="E17" s="7">
         <v>2</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="8">
         <v>200</v>
       </c>
-      <c r="G17" s="8">
+      <c r="G17" s="5">
         <f t="shared" si="0"/>
         <v>400</v>
       </c>
-      <c r="H17" s="6" t="s">
+      <c r="H17" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I17" s="6" t="s">
+      <c r="I17" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J17" s="6" t="s">
+      <c r="J17" s="7" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="4">
+      <c r="A18" s="6">
         <v>45408</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="4">
         <v>17</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="7">
         <v>3</v>
       </c>
-      <c r="F18" s="7">
+      <c r="F18" s="8">
         <v>150</v>
       </c>
-      <c r="G18" s="8">
+      <c r="G18" s="5">
         <f t="shared" si="0"/>
         <v>450</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="4">
+      <c r="A19" s="6">
         <v>45412</v>
       </c>
-      <c r="B19" s="5">
+      <c r="B19" s="4">
         <v>18</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="6" t="s">
+      <c r="D19" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E19" s="6">
+      <c r="E19" s="7">
         <v>8</v>
       </c>
-      <c r="F19" s="7">
+      <c r="F19" s="8">
         <v>200</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="5">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="H19" s="6" t="s">
+      <c r="H19" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="I19" s="6" t="s">
+      <c r="I19" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="J19" s="6" t="s">
+      <c r="J19" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="4">
+      <c r="A20" s="6">
         <v>45415</v>
       </c>
-      <c r="B20" s="5">
+      <c r="B20" s="4">
         <v>19</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="D20" s="6" t="s">
+      <c r="D20" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E20" s="6">
+      <c r="E20" s="7">
         <v>5</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="8">
         <v>120</v>
       </c>
-      <c r="G20" s="8">
+      <c r="G20" s="5">
         <f t="shared" si="0"/>
         <v>600</v>
       </c>
-      <c r="H20" s="6" t="s">
+      <c r="H20" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I20" s="6" t="s">
+      <c r="I20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="J20" s="6" t="s">
+      <c r="J20" s="7" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10">
-      <c r="A21" s="4">
+      <c r="A21" s="6">
         <v>45419</v>
       </c>
-      <c r="B21" s="5">
+      <c r="B21" s="4">
         <v>20</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E21" s="6">
+      <c r="E21" s="7">
         <v>1</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F21" s="8">
         <v>100</v>
       </c>
-      <c r="G21" s="8">
+      <c r="G21" s="5">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="I21" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="J21" s="6" t="s">
+      <c r="J21" s="7" t="s">
         <v>28</v>
       </c>
     </row>

</xml_diff>